<commit_message>
export: always sort output (easier to test and to read)
</commit_message>
<xml_diff>
--- a/tests/resources/expected/data_dict.xlsx
+++ b/tests/resources/expected/data_dict.xlsx
@@ -49,106 +49,106 @@
     <t xml:space="preserve">Types_count</t>
   </si>
   <si>
+    <t xml:space="preserve">test_db1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oid : 25359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECT : 25359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> . building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string : 25359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> . coord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARRAY(float : 50714, null : 2) : 25359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> . street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> . zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">borough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cuisine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARRAY(OBJECT : 93463, null : 738) : 25359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date : 93463</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string : 93463</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer : 93450, null : 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restaurant_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_col2</t>
+  </si>
+  <si>
     <t xml:space="preserve">test_db2</t>
   </si>
   <si>
     <t xml:space="preserve">test_col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cuisine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string : 25359</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oid : 25359</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restaurant_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRAY(OBJECT : 93463, null : 738) : 25359</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> : date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date : 93463</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> : grade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string : 93463</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> : score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer : 93450, null : 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBJECT : 25359</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> . building</t>
-  </si>
-  <si>
-    <t xml:space="preserve">building</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> . street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> . zipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> . coord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRAY(float : 50714, null : 2) : 25359</t>
-  </si>
-  <si>
-    <t xml:space="preserve">borough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_db1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_col1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_col2</t>
   </si>
 </sst>
 </file>
@@ -528,16 +528,16 @@
   </sheetPr>
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I39" activeCellId="2" sqref="I12:I13 I25:I27 I39:I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -592,7 +592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -618,7 +618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -632,7 +632,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>25359</v>
@@ -641,10 +641,10 @@
         <v>100</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -655,10 +655,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>25359</v>
@@ -667,10 +667,10 @@
         <v>100</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -681,10 +681,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>25359</v>
@@ -693,10 +693,10 @@
         <v>100</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -707,19 +707,19 @@
         <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,19 +733,19 @@
         <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,22 +759,22 @@
         <v>10</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
@@ -785,22 +785,22 @@
         <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>25359</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>25359</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
@@ -811,22 +811,22 @@
         <v>10</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="H11" s="0" t="n">
+        <v>93463</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>368.56</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <v>25359</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
@@ -843,16 +843,16 @@
         <v>33</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>25359</v>
+        <v>93463</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>100</v>
+        <v>368.56</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
@@ -863,22 +863,22 @@
         <v>10</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>25359</v>
+        <v>93463</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>100</v>
+        <v>368.56</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
@@ -889,10 +889,10 @@
         <v>10</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>25359</v>
@@ -901,10 +901,10 @@
         <v>100</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
@@ -927,18 +927,18 @@
         <v>100</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>11</v>
@@ -956,15 +956,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>13</v>
@@ -982,21 +982,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>25359</v>
@@ -1005,24 +1005,24 @@
         <v>100</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>25359</v>
@@ -1031,24 +1031,24 @@
         <v>100</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D20" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>25359</v>
@@ -1057,7 +1057,7 @@
         <v>100</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,25 +1065,25 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D21" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,25 +1091,25 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D22" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,88 +1117,88 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>26</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>25359</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J24" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <v>25359</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="H25" s="0" t="n">
+        <v>93463</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>368.56</v>
+      </c>
+      <c r="J25" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="0" t="n">
-        <v>25359</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>32</v>
@@ -1207,56 +1207,56 @@
         <v>33</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>25359</v>
+        <v>93463</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>100</v>
+        <v>368.56</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D27" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>25359</v>
+        <v>93463</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>100</v>
+        <v>368.56</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D28" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>25359</v>
@@ -1265,18 +1265,18 @@
         <v>100</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>39</v>
@@ -1291,15 +1291,15 @@
         <v>100</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>42</v>
@@ -1320,12 +1320,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>42</v>
@@ -1346,12 +1346,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>42</v>
@@ -1360,7 +1360,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>25359</v>
@@ -1369,24 +1369,24 @@
         <v>100</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>25359</v>
@@ -1395,24 +1395,24 @@
         <v>100</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>25359</v>
@@ -1421,7 +1421,7 @@
         <v>100</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,25 +1429,25 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,25 +1455,25 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,85 +1481,85 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>26</v>
       </c>
       <c r="H37" s="0" t="n">
-        <v>93463</v>
+        <v>25359</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>368.56</v>
+        <v>100</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>25359</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J38" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <v>25359</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="J38" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D39" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="H39" s="0" t="n">
+        <v>93463</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>368.56</v>
+      </c>
+      <c r="J39" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H39" s="0" t="n">
-        <v>25359</v>
-      </c>
-      <c r="I39" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>42</v>
@@ -1571,56 +1571,56 @@
         <v>33</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>25359</v>
+        <v>93463</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>100</v>
+        <v>368.56</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>25359</v>
+        <v>93463</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>100</v>
+        <v>368.56</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>25359</v>
@@ -1629,15 +1629,15 @@
         <v>100</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>42</v>
@@ -1655,7 +1655,7 @@
         <v>100</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>